<commit_message>
.ods really resolved, tc speeded up
</commit_message>
<xml_diff>
--- a/data/entities/demo_today.xlsx
+++ b/data/entities/demo_today.xlsx
@@ -1723,11 +1723,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2081583240"/>
-        <c:axId val="2053471800"/>
+        <c:axId val="2074450680"/>
+        <c:axId val="2074447032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2081583240"/>
+        <c:axId val="2074450680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,12 +1762,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2053471800"/>
+        <c:crossAx val="2074447032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053471800"/>
+        <c:axId val="2074447032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1811,7 +1811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081583240"/>
+        <c:crossAx val="2074450680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2298,11 +2298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2084053208"/>
-        <c:axId val="2084057176"/>
+        <c:axId val="2074374920"/>
+        <c:axId val="2074370952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2084053208"/>
+        <c:axId val="2074374920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,12 +2337,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084057176"/>
+        <c:crossAx val="2074370952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2084057176"/>
+        <c:axId val="2074370952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2386,7 +2386,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084053208"/>
+        <c:crossAx val="2074374920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2873,11 +2873,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2084096760"/>
-        <c:axId val="2084100728"/>
+        <c:axId val="2074332616"/>
+        <c:axId val="2074328648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2084096760"/>
+        <c:axId val="2074332616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2912,12 +2912,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084100728"/>
+        <c:crossAx val="2074328648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2084100728"/>
+        <c:axId val="2074328648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2961,7 +2961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084096760"/>
+        <c:crossAx val="2074332616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>

<commit_message>
switched to .xlsx for MATLAB version 9.x
still switching back to .xls for MATLAB 8 and earlier
</commit_message>
<xml_diff>
--- a/data/entities/demo_today.xlsx
+++ b/data/entities/demo_today.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bresch/Documents/_GIT/climada_data/entities/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14820" tabRatio="766" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="766"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -15,8 +20,11 @@
     <sheet name="_measures_details" sheetId="5" r:id="rId6"/>
     <sheet name="_discounting_sheet" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -246,6 +254,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="G1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>OPTIONAL
+The unit of the intensity, e.g. m/s for wind or MMI for earthquake. Please use SI units wherever possible.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>OPTIONAL
+a free name, only used for annotation. Use only letters,  numbers and spaces, do not start with a letter.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A2" authorId="0">
       <text>
         <r>
@@ -269,6 +303,18 @@
             <family val="2"/>
           </rPr>
           <t>used to replace 1 for measure enforce building code (mapped 1to3)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>o show the effect, NOT a really good damage function.</t>
         </r>
       </text>
     </comment>
@@ -765,7 +811,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>Intensity</t>
   </si>
@@ -990,6 +1036,18 @@
   </si>
   <si>
     <t>TC</t>
+  </si>
+  <si>
+    <t>Intensity_unit</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>Tropical cyclone default</t>
+  </si>
+  <si>
+    <t>TC Building code</t>
   </si>
 </sst>
 </file>
@@ -998,12 +1056,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1062,8 +1120,13 @@
       <color indexed="81"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1097,6 +1160,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1140,7 +1209,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1149,7 +1218,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1168,6 +1236,11 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1245,6 +1318,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1394,7 +1472,7 @@
             <c:numRef>
               <c:f>damagefunctions!$C$2:$C$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -1505,7 +1583,7 @@
             <c:numRef>
               <c:f>damagefunctions!$D$2:$D$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -1604,7 +1682,7 @@
             <c:numRef>
               <c:f>damagefunctions!$E$2:$E$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -1646,11 +1724,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2093215992"/>
-        <c:axId val="2093219416"/>
+        <c:axId val="545677200"/>
+        <c:axId val="545681760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2093215992"/>
+        <c:axId val="545677200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,12 +1763,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093219416"/>
+        <c:crossAx val="545681760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2093219416"/>
+        <c:axId val="545681760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1734,7 +1812,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093215992"/>
+        <c:crossAx val="545677200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1968,7 +2046,7 @@
             <c:numRef>
               <c:f>damagefunctions!$C$11:$C$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -2079,7 +2157,7 @@
             <c:numRef>
               <c:f>damagefunctions!$D$11:$D$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -2178,7 +2256,7 @@
             <c:numRef>
               <c:f>damagefunctions!$E$11:$E$19</c:f>
               <c:numCache>
-                <c:formatCode>_(* #\'##0.000000_);_(* \(#\'##0.000000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -2220,11 +2298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2093261864"/>
-        <c:axId val="2093265288"/>
+        <c:axId val="546677232"/>
+        <c:axId val="546681792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2093261864"/>
+        <c:axId val="546677232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2259,12 +2337,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093265288"/>
+        <c:crossAx val="546681792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2093265288"/>
+        <c:axId val="546681792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2308,7 +2386,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093261864"/>
+        <c:crossAx val="546677232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2400,16 +2478,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2432,16 +2510,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2789,9 +2867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
@@ -2799,10 +2877,10 @@
     <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2821,11 +2899,11 @@
       <c r="F1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>26.933899</v>
       </c>
@@ -2846,11 +2924,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="21">
         <v>5139300504.6792002</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>26.957203</v>
       </c>
@@ -2871,11 +2949,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>26.783846</v>
       </c>
@@ -2896,11 +2974,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>26.645524000000002</v>
       </c>
@@ -2921,11 +2999,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>26.897796</v>
       </c>
@@ -2946,11 +3024,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>26.925359</v>
       </c>
@@ -2971,11 +3049,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>26.914767999999999</v>
       </c>
@@ -2996,11 +3074,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="21">
         <v>4648538819.2559605</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>26.853491000000002</v>
       </c>
@@ -3021,11 +3099,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>26.845099000000001</v>
       </c>
@@ -3046,11 +3124,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="21">
         <v>4657184266.3798704</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>26.826509999999999</v>
       </c>
@@ -3071,11 +3149,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>26.842772</v>
       </c>
@@ -3096,11 +3174,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="21">
         <v>4651025709.2825003</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>26.825904999999999</v>
       </c>
@@ -3121,11 +3199,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>26.804649999999999</v>
       </c>
@@ -3146,11 +3224,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="21">
         <v>4961290391.9390001</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>26.788648999999999</v>
       </c>
@@ -3171,11 +3249,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="21">
         <v>5438960829.5693903</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>26.704277000000001</v>
       </c>
@@ -3196,11 +3274,11 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="21">
         <v>4651450127.7348204</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>26.710049999999999</v>
       </c>
@@ -3221,11 +3299,11 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="21">
         <v>4800322701.0994797</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>26.755412</v>
       </c>
@@ -3246,11 +3324,11 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="21">
         <v>4653832934.1885204</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>26.678449000000001</v>
       </c>
@@ -3271,11 +3349,11 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="21">
         <v>4661009648.1131401</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>26.725649000000001</v>
       </c>
@@ -3296,11 +3374,11 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="21">
         <v>4648800543.9682198</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>26.720599</v>
       </c>
@@ -3321,11 +3399,11 @@
       <c r="F21" s="1">
         <v>1</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="21">
         <v>4649451965.6613197</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>26.71255</v>
       </c>
@@ -3346,11 +3424,11 @@
       <c r="F22" s="1">
         <v>1</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="21">
         <v>4648559312.6040897</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>26.664899999999999</v>
       </c>
@@ -3371,11 +3449,11 @@
       <c r="F23" s="1">
         <v>1</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="21">
         <v>4728611180.8810101</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>26.664698999999999</v>
       </c>
@@ -3396,11 +3474,11 @@
       <c r="F24" s="1">
         <v>1</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="21">
         <v>4657477654.7297096</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>26.663149000000001</v>
       </c>
@@ -3421,11 +3499,11 @@
       <c r="F25" s="1">
         <v>1</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="21">
         <v>4648537081.1613503</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>26.668749999999999</v>
       </c>
@@ -3446,11 +3524,11 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="21">
         <v>4648940804.1615105</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>26.638517</v>
       </c>
@@ -3471,11 +3549,11 @@
       <c r="F27" s="1">
         <v>1</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="21">
         <v>4648357404.0137701</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>26.59309</v>
       </c>
@@ -3496,11 +3574,11 @@
       <c r="F28" s="1">
         <v>1</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="21">
         <v>4702738672.44872</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>26.617449000000001</v>
       </c>
@@ -3521,11 +3599,11 @@
       <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="21">
         <v>4652378148.9963999</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>26.620079</v>
       </c>
@@ -3546,11 +3624,11 @@
       <c r="F30" s="1">
         <v>1</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>26.596795</v>
       </c>
@@ -3571,11 +3649,11 @@
       <c r="F31" s="1">
         <v>1</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="21">
         <v>4681799806.2101603</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>26.577048999999999</v>
       </c>
@@ -3596,11 +3674,11 @@
       <c r="F32" s="1">
         <v>1</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="21">
         <v>4849820094.44631</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>26.524584999999998</v>
       </c>
@@ -3621,11 +3699,11 @@
       <c r="F33" s="1">
         <v>1</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="21">
         <v>4958704187.9946203</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>26.524158</v>
       </c>
@@ -3646,11 +3724,11 @@
       <c r="F34" s="1">
         <v>1</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="21">
         <v>4700541195.3858604</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>26.523737000000001</v>
       </c>
@@ -3671,11 +3749,11 @@
       <c r="F35" s="1">
         <v>1</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="21">
         <v>4648479198.5686197</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>26.520284</v>
       </c>
@@ -3696,11 +3774,11 @@
       <c r="F36" s="1">
         <v>1</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="21">
         <v>4693012294.9874296</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>26.547349000000001</v>
       </c>
@@ -3721,11 +3799,11 @@
       <c r="F37" s="1">
         <v>1</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>26.463398999999999</v>
       </c>
@@ -3746,11 +3824,11 @@
       <c r="F38" s="1">
         <v>1</v>
       </c>
-      <c r="G38" s="22">
+      <c r="G38" s="21">
         <v>4658942386.6735201</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>26.459050000000001</v>
       </c>
@@ -3771,11 +3849,11 @@
       <c r="F39" s="1">
         <v>1</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G39" s="21">
         <v>4648115411.3237801</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>26.455580000000001</v>
       </c>
@@ -3796,11 +3874,11 @@
       <c r="F40" s="1">
         <v>1</v>
       </c>
-      <c r="G40" s="22">
+      <c r="G40" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>26.453699</v>
       </c>
@@ -3821,11 +3899,11 @@
       <c r="F41" s="1">
         <v>1</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G41" s="21">
         <v>9034864234.9035301</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>26.449998999999998</v>
       </c>
@@ -3846,11 +3924,11 @@
       <c r="F42" s="1">
         <v>1</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="21">
         <v>4813012085.2491903</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>26.397299</v>
       </c>
@@ -3871,11 +3949,11 @@
       <c r="F43" s="1">
         <v>1</v>
       </c>
-      <c r="G43" s="22">
+      <c r="G43" s="21">
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>26.4084</v>
       </c>
@@ -3896,11 +3974,11 @@
       <c r="F44" s="1">
         <v>1</v>
       </c>
-      <c r="G44" s="22">
+      <c r="G44" s="21">
         <v>6762158257.6236</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>26.408750000000001</v>
       </c>
@@ -3921,11 +3999,11 @@
       <c r="F45" s="1">
         <v>1</v>
       </c>
-      <c r="G45" s="22">
+      <c r="G45" s="21">
         <v>4653572219.9963903</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>26.379113</v>
       </c>
@@ -3946,11 +4024,11 @@
       <c r="F46" s="1">
         <v>1</v>
       </c>
-      <c r="G46" s="22">
+      <c r="G46" s="21">
         <v>5313371933.3403101</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>26.3809</v>
       </c>
@@ -3971,11 +4049,11 @@
       <c r="F47" s="1">
         <v>1</v>
       </c>
-      <c r="G47" s="22">
+      <c r="G47" s="21">
         <v>4662182013.1408501</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>26.349067999999999</v>
       </c>
@@ -3996,11 +4074,11 @@
       <c r="F48" s="1">
         <v>1</v>
       </c>
-      <c r="G48" s="22">
+      <c r="G48" s="21">
         <v>4666138563.2157402</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>26.346349</v>
       </c>
@@ -4021,11 +4099,11 @@
       <c r="F49" s="1">
         <v>1</v>
       </c>
-      <c r="G49" s="22">
+      <c r="G49" s="21">
         <v>4728552813.2386103</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>26.348015</v>
       </c>
@@ -4046,11 +4124,11 @@
       <c r="F50" s="1">
         <v>1</v>
       </c>
-      <c r="G50" s="22">
+      <c r="G50" s="21">
         <v>4650520449.2202196</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>26.347957000000001</v>
       </c>
@@ -4071,40 +4149,35 @@
       <c r="F51" s="1">
         <v>1</v>
       </c>
-      <c r="G51" s="22">
+      <c r="G51" s="21">
         <v>4658604610.2166901</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4120,383 +4193,500 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="26">
-        <v>1</v>
-      </c>
-      <c r="B2" s="26">
-        <v>0</v>
-      </c>
-      <c r="C2" s="26">
-        <v>0</v>
-      </c>
-      <c r="D2" s="26">
-        <v>0</v>
-      </c>
-      <c r="E2" s="26">
+      <c r="G1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0</v>
+      </c>
+      <c r="D2" s="28">
+        <v>0</v>
+      </c>
+      <c r="E2" s="28">
+        <f>C2*D2</f>
         <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="26">
-        <v>1</v>
-      </c>
-      <c r="B3" s="26">
+      <c r="G2" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25">
         <v>20</v>
       </c>
-      <c r="C3" s="26">
-        <f t="shared" ref="C3:C10" si="0">E3/D3</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="26">
+      <c r="C3" s="28">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="28">
+        <f t="shared" ref="E3:E10" si="0">C3*D3</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="26">
-        <v>1</v>
-      </c>
-      <c r="B4" s="26">
+      <c r="G3" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="25">
         <v>30</v>
       </c>
-      <c r="C4" s="26">
-        <f t="shared" si="0"/>
+      <c r="C4" s="28">
         <v>2.1857142857142856E-2</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="28">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="28">
+        <f t="shared" si="0"/>
         <v>9.1799999999999998E-4</v>
       </c>
       <c r="F4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="26">
-        <v>1</v>
-      </c>
-      <c r="B5" s="26">
+      <c r="G4" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="25">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25">
         <v>40</v>
       </c>
-      <c r="C5" s="26">
-        <f t="shared" si="0"/>
+      <c r="C5" s="28">
         <v>3.5887499999999996E-2</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="28">
         <v>0.16</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="28">
+        <f t="shared" si="0"/>
         <v>5.7419999999999997E-3</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="26">
-        <v>1</v>
-      </c>
-      <c r="B6" s="26">
+      <c r="G5" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="25">
+        <v>1</v>
+      </c>
+      <c r="B6" s="25">
         <v>50</v>
       </c>
-      <c r="C6" s="26">
-        <f t="shared" si="0"/>
+      <c r="C6" s="28">
         <v>5.3977415307402764E-2</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="28">
         <v>0.39850000000000002</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="28">
+        <f t="shared" si="0"/>
         <v>2.1510000000000001E-2</v>
       </c>
       <c r="F6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="26">
-        <v>1</v>
-      </c>
-      <c r="B7" s="26">
+      <c r="G6" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="25">
+        <v>1</v>
+      </c>
+      <c r="B7" s="25">
         <v>60</v>
       </c>
-      <c r="C7" s="26">
-        <f t="shared" si="0"/>
+      <c r="C7" s="28">
         <v>0.10353424657534246</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="28">
         <v>0.65700000000000003</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="28">
+        <f t="shared" si="0"/>
         <v>6.8021999999999999E-2</v>
       </c>
       <c r="F7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="26">
-        <v>1</v>
-      </c>
-      <c r="B8" s="26">
+      <c r="G7" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="25">
+        <v>1</v>
+      </c>
+      <c r="B8" s="25">
         <v>70</v>
       </c>
-      <c r="C8" s="26">
-        <f t="shared" si="0"/>
+      <c r="C8" s="28">
         <v>0.18041399999999999</v>
       </c>
-      <c r="D8" s="26">
-        <v>1</v>
-      </c>
-      <c r="E8" s="26">
+      <c r="D8" s="28">
+        <v>1</v>
+      </c>
+      <c r="E8" s="28">
+        <f t="shared" si="0"/>
         <v>0.18041399999999999</v>
       </c>
       <c r="F8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="26">
-        <v>1</v>
-      </c>
-      <c r="B9" s="26">
+      <c r="G8" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="25">
+        <v>1</v>
+      </c>
+      <c r="B9" s="25">
         <v>80</v>
       </c>
-      <c r="C9" s="26">
-        <f t="shared" si="0"/>
+      <c r="C9" s="28">
         <v>0.41079599999999999</v>
       </c>
-      <c r="D9" s="26">
-        <v>1</v>
-      </c>
-      <c r="E9" s="26">
+      <c r="D9" s="28">
+        <v>1</v>
+      </c>
+      <c r="E9" s="28">
+        <f t="shared" si="0"/>
         <v>0.41079599999999999</v>
       </c>
       <c r="F9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="26">
-        <v>1</v>
-      </c>
-      <c r="B10" s="26">
+      <c r="G9" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="25">
+        <v>1</v>
+      </c>
+      <c r="B10" s="25">
         <v>100</v>
       </c>
-      <c r="C10" s="26">
-        <f t="shared" si="0"/>
+      <c r="C10" s="28">
         <v>0.41079599999999999</v>
       </c>
-      <c r="D10" s="26">
-        <v>1</v>
-      </c>
-      <c r="E10" s="26">
+      <c r="D10" s="28">
+        <v>1</v>
+      </c>
+      <c r="E10" s="28">
+        <f t="shared" si="0"/>
         <v>0.41079599999999999</v>
       </c>
       <c r="F10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>3</v>
       </c>
       <c r="B11" s="4">
         <v>0</v>
       </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
+      <c r="C11" s="29">
+        <v>0</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0</v>
+      </c>
+      <c r="E11" s="30">
+        <f>C11*D11</f>
         <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>3</v>
       </c>
       <c r="B12" s="4">
         <v>20</v>
       </c>
-      <c r="C12" s="4">
-        <f t="shared" ref="C12:C19" si="1">E12/D12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="29">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="30">
+        <f t="shared" ref="E12:E19" si="1">C12*D12</f>
         <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>3</v>
       </c>
       <c r="B13" s="4">
         <v>30</v>
       </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
+      <c r="C13" s="29">
+        <v>0</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0</v>
+      </c>
+      <c r="E13" s="30">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F13" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>3</v>
       </c>
       <c r="B14" s="4">
         <v>40</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="29">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0.16</v>
+      </c>
+      <c r="E14" s="30">
         <f t="shared" si="1"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.16</v>
-      </c>
-      <c r="E14" s="8">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F14" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>3</v>
       </c>
       <c r="B15" s="4">
         <v>50</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="29">
+        <v>5.4054054054054057E-2</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0.37</v>
+      </c>
+      <c r="E15" s="30">
         <f t="shared" si="1"/>
-        <v>5.4054054054054057E-2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.37</v>
-      </c>
-      <c r="E15" s="8">
         <v>0.02</v>
       </c>
       <c r="F15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>3</v>
       </c>
       <c r="B16" s="4">
         <v>60</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="29">
+        <v>0.10461538461538462</v>
+      </c>
+      <c r="D16" s="29">
+        <v>0.65</v>
+      </c>
+      <c r="E16" s="30">
         <f t="shared" si="1"/>
-        <v>0.10461538461538462</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="E16" s="8">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="F16" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>3</v>
       </c>
       <c r="B17" s="4">
         <v>70</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="29">
+        <v>0.21176470588235294</v>
+      </c>
+      <c r="D17" s="29">
+        <v>0.85</v>
+      </c>
+      <c r="E17" s="30">
         <f t="shared" si="1"/>
-        <v>0.21176470588235294</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="E17" s="8">
         <v>0.18</v>
       </c>
       <c r="F17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>3</v>
       </c>
       <c r="B18" s="4">
         <v>80</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="29">
+        <v>0.4</v>
+      </c>
+      <c r="D18" s="29">
+        <v>1</v>
+      </c>
+      <c r="E18" s="30">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0.4</v>
-      </c>
       <c r="F18" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>3</v>
       </c>
       <c r="B19" s="4">
         <v>100</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="29">
+        <v>0.4</v>
+      </c>
+      <c r="D19" s="29">
+        <v>1</v>
+      </c>
+      <c r="E19" s="30">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0.4</v>
-      </c>
       <c r="F19" t="s">
         <v>74</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4505,11 +4695,6 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4521,7 +4706,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
@@ -4535,7 +4720,7 @@
     <col min="13" max="13" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4576,7 +4761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -4618,14 +4803,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <f>30000000*4*6*2.4</f>
         <v>1728000000</v>
       </c>
@@ -4660,7 +4845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -4703,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -4749,11 +4934,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4765,12 +4945,12 @@
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -4781,578 +4961,573 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2000</v>
       </c>
-      <c r="C2" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2001</v>
       </c>
-      <c r="C3" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2002</v>
       </c>
-      <c r="C4" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>2003</v>
       </c>
-      <c r="C5" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>2004</v>
       </c>
-      <c r="C6" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>2005</v>
       </c>
-      <c r="C7" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>2006</v>
       </c>
-      <c r="C8" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>2007</v>
       </c>
-      <c r="C9" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>2008</v>
       </c>
-      <c r="C10" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>2009</v>
       </c>
-      <c r="C11" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>2010</v>
       </c>
-      <c r="C12" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>2011</v>
       </c>
-      <c r="C13" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>2012</v>
       </c>
-      <c r="C14" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>2013</v>
       </c>
-      <c r="C15" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="C15" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>2014</v>
       </c>
-      <c r="C16" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>2015</v>
       </c>
-      <c r="C17" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="C17" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>2016</v>
       </c>
-      <c r="C18" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C18" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>2017</v>
       </c>
-      <c r="C19" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="C19" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>2018</v>
       </c>
-      <c r="C20" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="C20" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>2019</v>
       </c>
-      <c r="C21" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="C21" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>2020</v>
       </c>
-      <c r="C22" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="C22" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>2021</v>
       </c>
-      <c r="C23" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>2022</v>
       </c>
-      <c r="C24" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="C24" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>2023</v>
       </c>
-      <c r="C25" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="C25" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>2024</v>
       </c>
-      <c r="C26" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="C26" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>2025</v>
       </c>
-      <c r="C27" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="C27" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>2026</v>
       </c>
-      <c r="C28" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="C28" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>2027</v>
       </c>
-      <c r="C29" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="C29" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>2028</v>
       </c>
-      <c r="C30" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="C30" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>2029</v>
       </c>
-      <c r="C31" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="C31" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
         <v>2030</v>
       </c>
-      <c r="C32" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="C32" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
         <v>2031</v>
       </c>
-      <c r="C33" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="C33" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
         <v>2032</v>
       </c>
-      <c r="C34" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="C34" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
         <v>2033</v>
       </c>
-      <c r="C35" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="C35" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
         <v>2034</v>
       </c>
-      <c r="C36" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="C36" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
         <v>2035</v>
       </c>
-      <c r="C37" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="C37" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
         <v>2036</v>
       </c>
-      <c r="C38" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="C38" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <v>2037</v>
       </c>
-      <c r="C39" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="C39" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
         <v>2038</v>
       </c>
-      <c r="C40" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="C40" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
         <v>2039</v>
       </c>
-      <c r="C41" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="C41" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
         <v>2040</v>
       </c>
-      <c r="C42" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="C42" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
         <v>2041</v>
       </c>
-      <c r="C43" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="C43" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
         <v>2042</v>
       </c>
-      <c r="C44" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="C44" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
         <v>2043</v>
       </c>
-      <c r="C45" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="C45" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <v>2044</v>
       </c>
-      <c r="C46" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="C46" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <v>2045</v>
       </c>
-      <c r="C47" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="C47" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
         <v>2046</v>
       </c>
-      <c r="C48" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="C48" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <v>2047</v>
       </c>
-      <c r="C49" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="C49" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
         <v>2048</v>
       </c>
-      <c r="C50" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="C50" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
         <v>2049</v>
       </c>
-      <c r="C51" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="C51" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
         <v>2050</v>
       </c>
-      <c r="C52" s="9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="C53" s="9"/>
+      <c r="C52" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C53" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5364,7 +5539,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -5374,12 +5549,12 @@
     <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -5393,76 +5568,76 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2010</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>657429034020.67725</v>
       </c>
       <c r="I4">
         <v>2010</v>
       </c>
-      <c r="J4" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K4" s="13">
+      <c r="J4" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K4" s="12">
         <f>B4</f>
         <v>657429034020.67725</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2030</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <f>K24</f>
         <v>976904961143.59058</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <f>B5/B4</f>
         <v>1.4859473959783549</v>
       </c>
       <c r="I5">
         <v>2011</v>
       </c>
-      <c r="J5" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K5" s="10">
+      <c r="J5" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K5" s="9">
         <f>K4*(1+J4)</f>
         <v>670577614701.09082</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I6">
         <v>2012</v>
       </c>
-      <c r="J6" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="J6" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K6" s="9">
         <f t="shared" ref="K6:K24" si="0">K5*(1+J5)</f>
         <v>683989166995.11267</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13" thickBot="1">
+    <row r="7" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="I7">
         <v>2013</v>
       </c>
-      <c r="J7" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="J7" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K7" s="9">
         <f t="shared" si="0"/>
         <v>697668950335.01489</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="13" thickBot="1">
+    <row r="8" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>1</v>
       </c>
       <c r="C8" t="s">
@@ -5471,240 +5646,235 @@
       <c r="I8">
         <v>2014</v>
       </c>
-      <c r="J8" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K8" s="10">
+      <c r="J8" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K8" s="9">
         <f t="shared" si="0"/>
         <v>711622329341.71521</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>57</v>
       </c>
       <c r="I9">
         <v>2015</v>
       </c>
-      <c r="J9" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K9" s="10">
+      <c r="J9" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K9" s="9">
         <f t="shared" si="0"/>
         <v>725854775928.54956</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <f>SUM(assets!C2:C51)</f>
         <v>657053294559.9104</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="23"/>
       <c r="I10">
         <v>2016</v>
       </c>
-      <c r="J10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K10" s="10">
+      <c r="J10" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K10" s="9">
         <f t="shared" si="0"/>
         <v>740371871447.12061</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I11">
         <v>2017</v>
       </c>
-      <c r="J11" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K11" s="10">
+      <c r="J11" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K11" s="9">
         <f t="shared" si="0"/>
         <v>755179308876.06299</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I12">
         <v>2018</v>
       </c>
-      <c r="J12" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K12" s="10">
+      <c r="J12" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K12" s="9">
         <f t="shared" si="0"/>
         <v>770282895053.58423</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I13">
         <v>2019</v>
       </c>
-      <c r="J13" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K13" s="10">
+      <c r="J13" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K13" s="9">
         <f t="shared" si="0"/>
         <v>785688552954.65588</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I14">
         <v>2020</v>
       </c>
-      <c r="J14" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K14" s="10">
+      <c r="J14" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K14" s="9">
         <f t="shared" si="0"/>
         <v>801402324013.74902</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I15">
         <v>2021</v>
       </c>
-      <c r="J15" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K15" s="10">
+      <c r="J15" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K15" s="9">
         <f t="shared" si="0"/>
         <v>817430370494.02405</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I16">
         <v>2022</v>
       </c>
-      <c r="J16" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K16" s="10">
+      <c r="J16" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K16" s="9">
         <f t="shared" si="0"/>
         <v>833778977903.90454</v>
       </c>
     </row>
-    <row r="17" spans="9:11">
+    <row r="17" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I17">
         <v>2023</v>
       </c>
-      <c r="J17" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K17" s="10">
+      <c r="J17" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K17" s="9">
         <f t="shared" si="0"/>
         <v>850454557461.98267</v>
       </c>
     </row>
-    <row r="18" spans="9:11">
+    <row r="18" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I18">
         <v>2024</v>
       </c>
-      <c r="J18" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K18" s="10">
+      <c r="J18" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K18" s="9">
         <f t="shared" si="0"/>
         <v>867463648611.22229</v>
       </c>
     </row>
-    <row r="19" spans="9:11">
+    <row r="19" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I19">
         <v>2025</v>
       </c>
-      <c r="J19" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K19" s="10">
+      <c r="J19" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K19" s="9">
         <f t="shared" si="0"/>
         <v>884812921583.44678</v>
       </c>
     </row>
-    <row r="20" spans="9:11">
+    <row r="20" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I20">
         <v>2026</v>
       </c>
-      <c r="J20" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K20" s="10">
+      <c r="J20" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K20" s="9">
         <f t="shared" si="0"/>
         <v>902509180015.11572</v>
       </c>
     </row>
-    <row r="21" spans="9:11">
+    <row r="21" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I21">
         <v>2027</v>
       </c>
-      <c r="J21" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K21" s="10">
+      <c r="J21" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K21" s="9">
         <f t="shared" si="0"/>
         <v>920559363615.41809</v>
       </c>
     </row>
-    <row r="22" spans="9:11">
+    <row r="22" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I22">
         <v>2028</v>
       </c>
-      <c r="J22" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K22" s="10">
+      <c r="J22" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K22" s="9">
         <f t="shared" si="0"/>
         <v>938970550887.72644</v>
       </c>
     </row>
-    <row r="23" spans="9:11">
+    <row r="23" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I23">
         <v>2029</v>
       </c>
-      <c r="J23" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K23" s="10">
+      <c r="J23" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K23" s="9">
         <f t="shared" si="0"/>
         <v>957749961905.48096</v>
       </c>
     </row>
-    <row r="24" spans="9:11">
+    <row r="24" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I24">
         <v>2030</v>
       </c>
-      <c r="J24" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="K24" s="10">
+      <c r="J24" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K24" s="9">
         <f t="shared" si="0"/>
         <v>976904961143.59058</v>
       </c>
     </row>
-    <row r="25" spans="9:11">
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="9:11">
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="9:11">
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="9:11">
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="9:11">
-      <c r="J29" s="9"/>
+    <row r="25" spans="9:11" x14ac:dyDescent="0.15">
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="9:11" x14ac:dyDescent="0.15">
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="9:11" x14ac:dyDescent="0.15">
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="9:11" x14ac:dyDescent="0.15">
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="9:11" x14ac:dyDescent="0.15">
+      <c r="J29" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5716,7 +5886,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -5724,156 +5894,156 @@
     <col min="4" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-    </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="11" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.2</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <f>B6*SUM(assets!C2:C51)*_measures_details!B7</f>
         <v>65705329455.991043</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>4000000</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="18">
         <f>_discounting_sheet!D4</f>
         <v>69405733.37838845</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
-      <c r="W13" s="13" t="e">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="W13" s="12" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>20000000</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>500000</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>500000</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>400000</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="18">
         <f>_discounting_sheet!F4</f>
         <v>43892006.68243596</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -5881,24 +6051,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>30000</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <f>B24^2*B25*2000</f>
         <v>540000000</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -5906,20 +6076,20 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="12">
         <f>B25*B27</f>
         <v>12000000</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="18">
         <f>_discounting_sheet!H4</f>
         <v>736217200.13516533</v>
       </c>
@@ -5928,11 +6098,6 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5944,7 +6109,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -5955,12 +6120,12 @@
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -5970,787 +6135,782 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>41</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="15"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2010</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <f>discount!C12</f>
         <v>0.02</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f t="shared" ref="D4:D23" si="0">C4+D5/(1+$B5)</f>
         <v>69405733.37838845</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <f>_measures_details!$B$16+_measures_details!$B$17+_measures_details!$B$18</f>
         <v>21000000</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <f t="shared" ref="F4:F23" si="1">E4+F5/(1+$B5)</f>
         <v>43892006.68243596</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <f>_measures_details!B26</f>
         <v>540000000</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="17">
         <f t="shared" ref="H4:H23" si="2">G4+H5/(1+$B5)</f>
         <v>736217200.13516533</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="K4" s="16"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2011</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <f>discount!C13</f>
         <v>0.02</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f t="shared" si="0"/>
         <v>66713848.045956217</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <f t="shared" si="1"/>
         <v>23349846.816084679</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <f t="shared" si="2"/>
         <v>200141544.13786864</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="K5" s="13"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2012</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <f>discount!C14</f>
         <v>0.02</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <f t="shared" si="0"/>
         <v>63968125.006875344</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <f t="shared" si="1"/>
         <v>22388843.752406374</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="17">
         <f t="shared" si="2"/>
         <v>191904375.02062601</v>
       </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="K6" s="13"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2013</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <f>discount!C15</f>
         <v>0.02</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <f t="shared" si="0"/>
         <v>61167487.507012852</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <f t="shared" si="1"/>
         <v>21408620.627454501</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="17">
         <f t="shared" si="2"/>
         <v>183502462.52103853</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="K7" s="13"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2014</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <f>discount!C16</f>
         <v>0.02</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <f t="shared" si="0"/>
         <v>58310837.257153109</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <f t="shared" si="1"/>
         <v>20408793.04000359</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <f t="shared" si="2"/>
         <v>174932511.77145931</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="K8" s="13"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2015</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <f>discount!C17</f>
         <v>0.02</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <f t="shared" si="0"/>
         <v>55397054.002296172</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <f t="shared" si="1"/>
         <v>19388968.900803663</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <f t="shared" si="2"/>
         <v>166191162.00688851</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="K9" s="13"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2016</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <f>discount!C18</f>
         <v>0.02</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <f t="shared" si="0"/>
         <v>52424995.082342096</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <f t="shared" si="1"/>
         <v>18348748.278819736</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <f t="shared" si="2"/>
         <v>157274985.24702629</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="K10" s="13"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2017</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <f>discount!C19</f>
         <v>0.02</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <f t="shared" si="0"/>
         <v>49393494.983988941</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <f t="shared" si="1"/>
         <v>17287723.244396131</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <f t="shared" si="2"/>
         <v>148180484.95196682</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="K11" s="13"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2018</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <f>discount!C20</f>
         <v>0.02</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <f t="shared" si="0"/>
         <v>46301364.883668721</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <f t="shared" si="1"/>
         <v>16205477.709284054</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <f t="shared" si="2"/>
         <v>138904094.65100616</v>
       </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="K12" s="13"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2019</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <f>discount!C21</f>
         <v>0.02</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <f t="shared" si="0"/>
         <v>43147392.181342095</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <f t="shared" si="1"/>
         <v>15101587.263469735</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="17">
         <f t="shared" si="2"/>
         <v>129442176.54402629</v>
       </c>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="K13" s="13"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2020</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <f>discount!C22</f>
         <v>0.02</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <f t="shared" si="0"/>
         <v>39930340.024968937</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <f t="shared" si="1"/>
         <v>13975619.008739131</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="17">
         <f t="shared" si="2"/>
         <v>119791020.07490681</v>
       </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="K14" s="13"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="13"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2021</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <f>discount!C23</f>
         <v>0.02</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <f t="shared" si="0"/>
         <v>36648946.825468317</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <f t="shared" si="1"/>
         <v>12827131.388913913</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="17">
         <f t="shared" si="2"/>
         <v>109946840.47640495</v>
       </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="K15" s="13"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="13"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2022</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="15">
         <f>discount!C24</f>
         <v>0.02</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="17">
         <f t="shared" si="0"/>
         <v>33301925.761977687</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <f t="shared" si="1"/>
         <v>11655674.016692191</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="17">
         <f t="shared" si="2"/>
         <v>99905777.285933048</v>
       </c>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="K16" s="13"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2023</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="15">
         <f>discount!C25</f>
         <v>0.02</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <f t="shared" si="0"/>
         <v>29887964.277217243</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="17">
         <f t="shared" si="1"/>
         <v>10460787.497026036</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="17">
         <f t="shared" si="2"/>
         <v>89663892.831651717</v>
       </c>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="K17" s="13"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2024</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="15">
         <f>discount!C26</f>
         <v>0.02</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="17">
         <f t="shared" si="0"/>
         <v>26405723.56276159</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="17">
         <f t="shared" si="1"/>
         <v>9242003.2469665557</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="17">
         <f t="shared" si="2"/>
         <v>79217170.688284755</v>
       </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="14"/>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="K18" s="13"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="13"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2025</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="15">
         <f>discount!C27</f>
         <v>0.02</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="17">
         <f t="shared" si="0"/>
         <v>22853838.034016822</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="17">
         <f t="shared" si="1"/>
         <v>7998843.311905887</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="17">
         <f t="shared" si="2"/>
         <v>68561514.102050453</v>
       </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="K19" s="13"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="13"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2026</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="15">
         <f>discount!C28</f>
         <v>0.02</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="17">
         <f t="shared" si="0"/>
         <v>19230914.794697158</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <f t="shared" si="1"/>
         <v>6730820.1781440051</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="17">
         <f t="shared" si="2"/>
         <v>57692744.384091474</v>
       </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="14"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="K20" s="13"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="13"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2027</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="15">
         <f>discount!C29</f>
         <v>0.02</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="17">
         <f t="shared" si="0"/>
         <v>15535533.090591099</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="17">
         <f t="shared" si="1"/>
         <v>5437436.5817068852</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="17">
         <f t="shared" si="2"/>
         <v>46606599.271773301</v>
       </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="14"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="K21" s="13"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2028</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="15">
         <f>discount!C30</f>
         <v>0.02</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <f t="shared" si="0"/>
         <v>11766243.752402922</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="17">
         <f t="shared" si="1"/>
         <v>4118185.3133410225</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="17">
         <f t="shared" si="2"/>
         <v>35298731.257208765</v>
       </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="K22" s="13"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="13"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2029</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="15">
         <f>discount!C31</f>
         <v>0.02</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="17">
         <f t="shared" si="0"/>
         <v>7921568.6274509802</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="17">
         <f t="shared" si="1"/>
         <v>2772549.0196078429</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="17">
         <f t="shared" si="2"/>
         <v>23764705.882352941</v>
       </c>
-      <c r="K23" s="14"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="14"/>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="K23" s="13"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>2030</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="15">
         <f>discount!C32</f>
         <v>0.02</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <f>_measures_details!$B$11</f>
         <v>4000000</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="17">
         <f>C24</f>
         <v>4000000</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <f>_measures_details!$B$17+_measures_details!$B$18+_measures_details!$B$19</f>
         <v>1400000</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="17">
         <f>E24</f>
         <v>1400000</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="9">
         <f>_measures_details!$B$28</f>
         <v>12000000</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="17">
         <f>G24</f>
         <v>12000000</v>
       </c>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="14"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>